<commit_message>
GPT was changed to LLM
</commit_message>
<xml_diff>
--- a/data/gold_standard_comparison/Triples_GPT_for_comparison.xlsx
+++ b/data/gold_standard_comparison/Triples_GPT_for_comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Workspace\SCAI_code\data\GoldSt_comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Workspace\SCAI_code\data\gold_standard_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51BB09A0-5B76-4DC1-B60F-1113F602966D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BEBB4A-6BA2-42D0-8FC5-52822DED89DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4966,7 +4966,7 @@
     <t>Source</t>
   </si>
   <si>
-    <t>GPT</t>
+    <t>LLM</t>
   </si>
 </sst>
 </file>
@@ -5331,8 +5331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G979"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B965" sqref="B965"/>
+    <sheetView tabSelected="1" topLeftCell="A956" workbookViewId="0">
+      <selection activeCell="I976" sqref="I976"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>